<commit_message>
Update ClickbankAdapter.js v1.6.0 and Rollback ParamMapLoaderCsv.js v1.2.0 and Create OfferMapLoaderCsv.js v1.0.0
</commit_message>
<xml_diff>
--- a/ClicckbankAdapter.js_url-tests.xlsx
+++ b/ClicckbankAdapter.js_url-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50f1f96246d526ec/Projetos/google-auth-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{462A1F39-A2A5-4631-AFE2-875747DF1502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0A2305C-04FF-49C0-9725-071782B378F4}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{462A1F39-A2A5-4631-AFE2-875747DF1502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F73AB452-421F-403C-A4FF-CF7E6DD5A0EF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{C465AEB8-D683-4A4D-BA7A-B7536DDAEE04}"/>
+    <workbookView xWindow="-96" yWindow="12600" windowWidth="23232" windowHeight="12696" xr2:uid="{C465AEB8-D683-4A4D-BA7A-B7536DDAEE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -923,19 +923,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6901C6-15D0-4E12-8CF2-26CBC23EB90E}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:D7"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.5546875" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="71.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="103.6640625" style="1" customWidth="1"/>
     <col min="5" max="9" width="35.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BA7C3A-C923-42F7-920D-33A6FAF15F86}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>